<commit_message>
Body size measurements and sample updates
</commit_message>
<xml_diff>
--- a/Background/sample_tracker.xlsx
+++ b/Background/sample_tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsasaki/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjbur\Desktop\Lab_projects\E_herdmani_size_morphs\Background\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F08FB9-7C1F-BD41-95C7-66BCC1CF3D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C27A3A-261E-4CA1-8E7D-81CF8DEE5892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="820" windowWidth="28100" windowHeight="17440" xr2:uid="{10805E3D-6642-F64C-9AAD-30ABC1E49B30}"/>
+    <workbookView xWindow="9708" yWindow="12" windowWidth="13332" windowHeight="12048" xr2:uid="{10805E3D-6642-F64C-9AAD-30ABC1E49B30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -456,12 +456,12 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="15.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,35 +475,43 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="15.6">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2">
+        <v>30</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="15.6">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="15.6">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>30</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="15.6">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>15</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>

</xml_diff>

<commit_message>
Lab notebook and size images
</commit_message>
<xml_diff>
--- a/Background/sample_tracker.xlsx
+++ b/Background/sample_tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjbur\Desktop\Lab_projects\E_herdmani_size_morphs\Background\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C27A3A-261E-4CA1-8E7D-81CF8DEE5892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F298D9-7CD6-46CE-93FD-A95483B247A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9708" yWindow="12" windowWidth="13332" windowHeight="12048" xr2:uid="{10805E3D-6642-F64C-9AAD-30ABC1E49B30}"/>
+    <workbookView xWindow="8340" yWindow="1368" windowWidth="13332" windowHeight="12048" xr2:uid="{10805E3D-6642-F64C-9AAD-30ABC1E49B30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -456,7 +456,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15"/>
@@ -482,7 +482,9 @@
       <c r="B2" s="2">
         <v>30</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2">
+        <v>30</v>
+      </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="15.6">
@@ -503,7 +505,9 @@
         <v>30</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15.6">
       <c r="A5" s="1" t="s">

</xml_diff>